<commit_message>
Planilla de metricas probador terminada
Planilla de metricas probador terminada: Agrego los tiempos faltantes.
</commit_message>
<xml_diff>
--- a/Documentacion/Probador/Probador - Planilla de Métricas V2.1.xlsx
+++ b/Documentacion/Probador/Probador - Planilla de Métricas V2.1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1053,37 +1053,38 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1093,26 +1094,11 @@
     <xf numFmtId="49" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1124,30 +1110,75 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC00000"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -1225,7 +1256,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="es-AR"/>
   <c:roundedCorners val="1"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
@@ -1236,8 +1267,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.3565974707706982E-2"/>
           <c:y val="7.4074152627750078E-2"/>
-          <c:w val="0.40158680164979443"/>
-          <c:h val="0.85185169474450095"/>
+          <c:w val="0.40158680164979454"/>
+          <c:h val="0.85185169474450106"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -1325,7 +1356,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Métricas!$B$48:$B$53</c:f>
+              <c:f>Métricas!$B$48:$D$53</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1351,10 +1382,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Métricas!$C$48:$C$53</c:f>
+              <c:f>Métricas!$F$48:$F$53</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.22500000000000009</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9999999999999843E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.4999999999999761E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0000000000000037E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.60000000000000031</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1374,6 +1423,17 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US"/>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
@@ -1381,7 +1441,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1392,15 +1452,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1677,7 +1737,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1687,11 +1747,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -1707,23 +1767,23 @@
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="92" t="s">
+      <c r="C1" s="123"/>
+      <c r="D1" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="123"/>
+      <c r="K1" s="123"/>
+      <c r="L1" s="123"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="123"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1940,15 +2000,15 @@
       <c r="E8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="98"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="93"/>
-      <c r="N8" s="93"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="123"/>
+      <c r="I8" s="123"/>
+      <c r="J8" s="123"/>
+      <c r="K8" s="123"/>
+      <c r="L8" s="123"/>
+      <c r="M8" s="123"/>
+      <c r="N8" s="123"/>
       <c r="O8" s="7"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="14"/>
@@ -1967,21 +2027,25 @@
       <c r="B9" s="16">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="18" t="str">
+      <c r="C9" s="17">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D9" s="25">
+        <v>0.96527777777777779</v>
+      </c>
+      <c r="E9" s="18">
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
-        <v>Completar</v>
+        <v>6.9444444444444198E-3</v>
       </c>
-      <c r="F9" s="99"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="93"/>
-      <c r="L9" s="93"/>
-      <c r="M9" s="93"/>
-      <c r="N9" s="93"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="123"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="123"/>
+      <c r="M9" s="123"/>
+      <c r="N9" s="123"/>
       <c r="O9" s="15"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="22"/>
@@ -2067,15 +2131,15 @@
       <c r="E12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="98"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="93"/>
-      <c r="I12" s="93"/>
-      <c r="J12" s="93"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="93"/>
-      <c r="M12" s="93"/>
-      <c r="N12" s="93"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="123"/>
+      <c r="J12" s="123"/>
+      <c r="K12" s="123"/>
+      <c r="L12" s="123"/>
+      <c r="M12" s="123"/>
+      <c r="N12" s="123"/>
       <c r="O12" s="7"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="14"/>
@@ -2104,15 +2168,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>1.041666666666663E-2</v>
       </c>
-      <c r="F13" s="99"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
-      <c r="M13" s="93"/>
-      <c r="N13" s="93"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="123"/>
+      <c r="J13" s="123"/>
+      <c r="K13" s="123"/>
+      <c r="L13" s="123"/>
+      <c r="M13" s="123"/>
+      <c r="N13" s="123"/>
       <c r="O13" s="15"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="22"/>
@@ -2186,31 +2250,31 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="123" t="s">
+      <c r="B16" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="125" t="s">
+      <c r="C16" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="126"/>
-      <c r="E16" s="126"/>
-      <c r="F16" s="119" t="s">
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="120"/>
-      <c r="H16" s="118" t="s">
+      <c r="G16" s="116"/>
+      <c r="H16" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="101"/>
-      <c r="J16" s="101"/>
-      <c r="K16" s="119" t="s">
+      <c r="I16" s="111"/>
+      <c r="J16" s="111"/>
+      <c r="K16" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="L16" s="120"/>
-      <c r="M16" s="121" t="s">
+      <c r="L16" s="116"/>
+      <c r="M16" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="N16" s="113" t="s">
+      <c r="N16" s="112" t="s">
         <v>5</v>
       </c>
       <c r="O16" s="7"/>
@@ -2228,10 +2292,10 @@
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="124"/>
-      <c r="C17" s="127"/>
-      <c r="D17" s="128"/>
-      <c r="E17" s="128"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
       <c r="F17" s="26" t="s">
         <v>15</v>
       </c>
@@ -2253,8 +2317,8 @@
       <c r="L17" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M17" s="122"/>
-      <c r="N17" s="114"/>
+      <c r="M17" s="118"/>
+      <c r="N17" s="113"/>
       <c r="O17" s="7"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="14"/>
@@ -2274,11 +2338,11 @@
         <f t="shared" ref="B18:B36" si="0">ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="115" t="s">
+      <c r="C18" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="129"/>
-      <c r="E18" s="130"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="107"/>
       <c r="F18" s="31">
         <v>5</v>
       </c>
@@ -2327,11 +2391,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C19" s="115" t="s">
+      <c r="C19" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="101"/>
-      <c r="E19" s="101"/>
+      <c r="D19" s="111"/>
+      <c r="E19" s="111"/>
       <c r="F19" s="31">
         <v>80</v>
       </c>
@@ -2380,11 +2444,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="115" t="s">
+      <c r="C20" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
+      <c r="D20" s="111"/>
+      <c r="E20" s="111"/>
       <c r="F20" s="73">
         <v>15</v>
       </c>
@@ -2433,9 +2497,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="115"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="101"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="111"/>
       <c r="F21" s="31"/>
       <c r="G21" s="78"/>
       <c r="H21" s="74"/>
@@ -2470,9 +2534,9 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="116"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="117"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="93"/>
       <c r="F22" s="67"/>
       <c r="G22" s="78"/>
       <c r="H22" s="74"/>
@@ -2507,9 +2571,9 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="107"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="101"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="111"/>
+      <c r="E23" s="111"/>
       <c r="F23" s="40"/>
       <c r="G23" s="78"/>
       <c r="H23" s="74"/>
@@ -2544,9 +2608,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="107"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="101"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="111"/>
       <c r="F24" s="40"/>
       <c r="G24" s="78"/>
       <c r="H24" s="74"/>
@@ -2581,9 +2645,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="107"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="101"/>
+      <c r="C25" s="108"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="111"/>
       <c r="F25" s="40"/>
       <c r="G25" s="78"/>
       <c r="H25" s="74"/>
@@ -2618,9 +2682,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C26" s="107"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="101"/>
+      <c r="C26" s="108"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="111"/>
       <c r="F26" s="40"/>
       <c r="G26" s="78"/>
       <c r="H26" s="74"/>
@@ -2655,9 +2719,9 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C27" s="107"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="101"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="111"/>
       <c r="F27" s="40"/>
       <c r="G27" s="78"/>
       <c r="H27" s="74"/>
@@ -2692,9 +2756,9 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C28" s="107"/>
-      <c r="D28" s="108"/>
-      <c r="E28" s="109"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="109"/>
+      <c r="E28" s="110"/>
       <c r="F28" s="40"/>
       <c r="G28" s="78"/>
       <c r="H28" s="74"/>
@@ -2729,9 +2793,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C29" s="107"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="101"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="111"/>
+      <c r="E29" s="111"/>
       <c r="F29" s="40"/>
       <c r="G29" s="78"/>
       <c r="H29" s="74"/>
@@ -2766,9 +2830,9 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C30" s="107"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="101"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="111"/>
+      <c r="E30" s="111"/>
       <c r="F30" s="40"/>
       <c r="G30" s="78"/>
       <c r="H30" s="74"/>
@@ -2803,9 +2867,9 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C31" s="107"/>
-      <c r="D31" s="108"/>
-      <c r="E31" s="109"/>
+      <c r="C31" s="108"/>
+      <c r="D31" s="109"/>
+      <c r="E31" s="110"/>
       <c r="F31" s="73"/>
       <c r="G31" s="78"/>
       <c r="H31" s="74"/>
@@ -2840,9 +2904,9 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C32" s="116"/>
-      <c r="D32" s="117"/>
-      <c r="E32" s="117"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="93"/>
+      <c r="E32" s="93"/>
       <c r="F32" s="82"/>
       <c r="G32" s="78"/>
       <c r="H32" s="74"/>
@@ -2877,9 +2941,9 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C33" s="116"/>
-      <c r="D33" s="117"/>
-      <c r="E33" s="117"/>
+      <c r="C33" s="92"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
       <c r="F33" s="82"/>
       <c r="G33" s="78"/>
       <c r="H33" s="74"/>
@@ -2914,9 +2978,9 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C34" s="116"/>
-      <c r="D34" s="117"/>
-      <c r="E34" s="117"/>
+      <c r="C34" s="92"/>
+      <c r="D34" s="93"/>
+      <c r="E34" s="93"/>
       <c r="F34" s="82"/>
       <c r="G34" s="78"/>
       <c r="H34" s="74"/>
@@ -2988,9 +3052,9 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C36" s="107"/>
-      <c r="D36" s="108"/>
-      <c r="E36" s="109"/>
+      <c r="C36" s="108"/>
+      <c r="D36" s="109"/>
+      <c r="E36" s="110"/>
       <c r="F36" s="40"/>
       <c r="G36" s="78"/>
       <c r="H36" s="74"/>
@@ -3021,12 +3085,12 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A37" s="7"/>
-      <c r="B37" s="131" t="s">
+      <c r="B37" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="106"/>
-      <c r="D37" s="106"/>
-      <c r="E37" s="106"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="98"/>
+      <c r="E37" s="98"/>
       <c r="F37" s="42">
         <f>IF(SUM(F18:F36)=0,"Completar",SUM(F18:F36))</f>
         <v>100</v>
@@ -3168,14 +3232,20 @@
       <c r="Y40" s="14"/>
       <c r="Z40" s="14"/>
     </row>
-    <row r="41" spans="1:26" ht="15.75" customHeight="1">
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A41" s="15"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="18" t="str">
+      <c r="B41" s="51">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C41" s="75">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="D41" s="25">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E41" s="18">
         <f>IFERROR(IF(OR(ISBLANK(C41),ISBLANK(D41)),"Completar",IF(D41&gt;=C41,D41-C41,"Error")),"Error")</f>
-        <v>Completar</v>
+        <v>6.9444444444444475E-3</v>
       </c>
       <c r="F41" s="15"/>
       <c r="G41" s="15"/>
@@ -3199,7 +3269,7 @@
       <c r="Y41" s="22"/>
       <c r="Z41" s="22"/>
     </row>
-    <row r="42" spans="1:26" ht="6" customHeight="1">
+    <row r="42" spans="1:26" ht="6" customHeight="1" thickBot="1">
       <c r="A42" s="20"/>
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
@@ -3259,16 +3329,16 @@
     </row>
     <row r="44" spans="1:26" ht="15" customHeight="1">
       <c r="A44" s="20"/>
-      <c r="B44" s="100" t="s">
+      <c r="B44" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="101"/>
-      <c r="D44" s="102"/>
-      <c r="E44" s="112">
+      <c r="C44" s="111"/>
+      <c r="D44" s="120"/>
+      <c r="E44" s="121">
         <f>M37</f>
         <v>96</v>
       </c>
-      <c r="F44" s="102"/>
+      <c r="F44" s="120"/>
       <c r="G44" s="53"/>
       <c r="H44" s="54"/>
       <c r="I44" s="54"/>
@@ -3292,16 +3362,16 @@
     </row>
     <row r="45" spans="1:26">
       <c r="A45" s="20"/>
-      <c r="B45" s="100" t="s">
+      <c r="B45" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="101"/>
-      <c r="D45" s="102"/>
-      <c r="E45" s="111">
+      <c r="C45" s="111"/>
+      <c r="D45" s="120"/>
+      <c r="E45" s="129">
         <f>IF(M37="Completar","Completar",IFERROR(M37/(N37*24),"Error"))</f>
         <v>48</v>
       </c>
-      <c r="F45" s="102"/>
+      <c r="F45" s="120"/>
       <c r="G45" s="56"/>
       <c r="H45" s="57"/>
       <c r="I45" s="57"/>
@@ -3325,16 +3395,16 @@
     </row>
     <row r="46" spans="1:26" ht="15" customHeight="1">
       <c r="A46" s="20"/>
-      <c r="B46" s="100" t="s">
+      <c r="B46" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="101"/>
-      <c r="D46" s="102"/>
-      <c r="E46" s="112">
+      <c r="C46" s="111"/>
+      <c r="D46" s="120"/>
+      <c r="E46" s="121">
         <f>IF(K37=0,0,IFERROR(ROUNDUP(K37/(M37/100),0),"Error"))</f>
         <v>0</v>
       </c>
-      <c r="F46" s="102"/>
+      <c r="F46" s="120"/>
       <c r="G46" s="56"/>
       <c r="H46" s="57"/>
       <c r="I46" s="57"/>
@@ -3358,16 +3428,16 @@
     </row>
     <row r="47" spans="1:26" ht="15" customHeight="1">
       <c r="A47" s="20"/>
-      <c r="B47" s="100" t="s">
+      <c r="B47" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="101"/>
-      <c r="D47" s="102"/>
-      <c r="E47" s="110">
+      <c r="C47" s="111"/>
+      <c r="D47" s="120"/>
+      <c r="E47" s="128">
         <f>IF(K37=0,0,IFERROR(K37/M37,"Error"))</f>
         <v>0</v>
       </c>
-      <c r="F47" s="102"/>
+      <c r="F47" s="120"/>
       <c r="G47" s="56"/>
       <c r="H47" s="57"/>
       <c r="I47" s="57"/>
@@ -3391,18 +3461,18 @@
     </row>
     <row r="48" spans="1:26" ht="15" customHeight="1">
       <c r="A48" s="20"/>
-      <c r="B48" s="100" t="s">
+      <c r="B48" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="101"/>
-      <c r="D48" s="102"/>
+      <c r="C48" s="111"/>
+      <c r="D48" s="120"/>
       <c r="E48" s="59">
         <f>E5</f>
         <v>3.125E-2</v>
       </c>
       <c r="F48" s="60">
         <f t="shared" ref="F48:F51" si="3">IF(E48="Completar",E48,IFERROR(E48/$E$54,"Error"))</f>
-        <v>0.25000000000000006</v>
+        <v>0.22500000000000009</v>
       </c>
       <c r="G48" s="56"/>
       <c r="H48" s="57"/>
@@ -3427,18 +3497,18 @@
     </row>
     <row r="49" spans="1:26" ht="15" customHeight="1">
       <c r="A49" s="20"/>
-      <c r="B49" s="100" t="s">
+      <c r="B49" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="101"/>
-      <c r="D49" s="102"/>
-      <c r="E49" s="59" t="str">
+      <c r="C49" s="111"/>
+      <c r="D49" s="120"/>
+      <c r="E49" s="59">
         <f>E9</f>
-        <v>Completar</v>
+        <v>6.9444444444444198E-3</v>
       </c>
-      <c r="F49" s="60" t="str">
+      <c r="F49" s="60">
         <f t="shared" si="3"/>
-        <v>Completar</v>
+        <v>4.9999999999999843E-2</v>
       </c>
       <c r="G49" s="56"/>
       <c r="H49" s="57"/>
@@ -3463,18 +3533,18 @@
     </row>
     <row r="50" spans="1:26" ht="15" customHeight="1">
       <c r="A50" s="20"/>
-      <c r="B50" s="100" t="s">
+      <c r="B50" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="C50" s="101"/>
-      <c r="D50" s="102"/>
+      <c r="C50" s="111"/>
+      <c r="D50" s="120"/>
       <c r="E50" s="59">
         <f>E13</f>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="F50" s="60">
         <f t="shared" si="3"/>
-        <v>8.3333333333333051E-2</v>
+        <v>7.4999999999999761E-2</v>
       </c>
       <c r="G50" s="56"/>
       <c r="H50" s="57"/>
@@ -3499,18 +3569,18 @@
     </row>
     <row r="51" spans="1:26" ht="15" customHeight="1">
       <c r="A51" s="20"/>
-      <c r="B51" s="100" t="s">
+      <c r="B51" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="101"/>
-      <c r="D51" s="102"/>
-      <c r="E51" s="59" t="str">
+      <c r="C51" s="111"/>
+      <c r="D51" s="120"/>
+      <c r="E51" s="59">
         <f>E41</f>
-        <v>Completar</v>
+        <v>6.9444444444444475E-3</v>
       </c>
-      <c r="F51" s="60" t="str">
+      <c r="F51" s="60">
         <f t="shared" si="3"/>
-        <v>Completar</v>
+        <v>5.0000000000000037E-2</v>
       </c>
       <c r="G51" s="56"/>
       <c r="H51" s="57"/>
@@ -3535,11 +3605,11 @@
     </row>
     <row r="52" spans="1:26" ht="15" customHeight="1">
       <c r="A52" s="20"/>
-      <c r="B52" s="100" t="s">
+      <c r="B52" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="C52" s="101"/>
-      <c r="D52" s="102"/>
+      <c r="C52" s="111"/>
+      <c r="D52" s="120"/>
       <c r="E52" s="59">
         <f>L37</f>
         <v>0</v>
@@ -3571,18 +3641,18 @@
     </row>
     <row r="53" spans="1:26" ht="15" customHeight="1">
       <c r="A53" s="20"/>
-      <c r="B53" s="100" t="s">
+      <c r="B53" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="C53" s="101"/>
-      <c r="D53" s="102"/>
+      <c r="C53" s="111"/>
+      <c r="D53" s="120"/>
       <c r="E53" s="59">
         <f>J37</f>
         <v>8.3333333333333343E-2</v>
       </c>
       <c r="F53" s="60">
         <f t="shared" si="4"/>
-        <v>0.66666666666666685</v>
+        <v>0.60000000000000031</v>
       </c>
       <c r="G53" s="56"/>
       <c r="H53" s="57"/>
@@ -3607,16 +3677,16 @@
     </row>
     <row r="54" spans="1:26" ht="15" customHeight="1">
       <c r="A54" s="20"/>
-      <c r="B54" s="105" t="s">
+      <c r="B54" s="127" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="106"/>
-      <c r="D54" s="104"/>
-      <c r="E54" s="103">
+      <c r="C54" s="98"/>
+      <c r="D54" s="126"/>
+      <c r="E54" s="125">
         <f>IF(COUNTIF(E48:E53,"Error")&gt;0,"Error",IF(SUM(E48:E53)=0,"Completar",SUM(E48:E53)))</f>
-        <v>0.12499999999999997</v>
+        <v>0.13888888888888884</v>
       </c>
-      <c r="F54" s="104"/>
+      <c r="F54" s="126"/>
       <c r="G54" s="61"/>
       <c r="H54" s="62"/>
       <c r="I54" s="62"/>
@@ -30436,37 +30506,13 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B43:N43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
     <mergeCell ref="B15:N15"/>
     <mergeCell ref="F12:N12"/>
     <mergeCell ref="F13:N13"/>
@@ -30483,31 +30529,55 @@
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="E45:F45"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B43:N43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
   </mergeCells>
-  <conditionalFormatting sqref="A37:XFD1048576 N36:XFD36 N20:N36 C3:C24 N25:XFD34 O35:XFD35 A1:B36 C25:M26 C27:I27 C28 F28:I28 C29:I34 J27:M34 D1:E17 D19:E24 L18:L36 G20:K36 C20:H20 F1:XFD24">
-    <cfRule type="cellIs" dxfId="3" priority="35" operator="equal">
+  <conditionalFormatting sqref="N36:XFD36 N20:N36 C3:C24 N25:XFD34 O35:XFD35 A1:B36 C25:M26 C27:I27 C28 F28:I28 C29:I34 J27:M34 D1:E17 D19:E24 L18:L36 G20:K36 C20:H20 F1:XFD24 A37:XFD1048576">
+    <cfRule type="cellIs" dxfId="5" priority="35" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37:XFD1048576 N36:XFD36 N20:N36 C3:C24 N25:XFD34 O35:XFD35 A1:B36 C25:M26 C27:I27 C28 F28:I28 C29:I34 J27:M34 D1:E17 D19:E24 L18:L36 G20:K36 C20:H20 F1:XFD24">
-    <cfRule type="cellIs" dxfId="2" priority="36" operator="equal">
+  <conditionalFormatting sqref="N36:XFD36 N20:N36 C3:C24 N25:XFD34 O35:XFD35 A1:B36 C25:M26 C27:I27 C28 F28:I28 C29:I34 J27:M34 D1:E17 D19:E24 L18:L36 G20:K36 C20:H20 F1:XFD24 A37:XFD1048576">
+    <cfRule type="cellIs" dxfId="4" priority="36" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36 F36:I36 K36:M36">
-    <cfRule type="cellIs" dxfId="1" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="27" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36 F36:I36 K36:M36">
-    <cfRule type="cellIs" dxfId="0" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="28" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>